<commit_message>
Mise à jour de certains champs de Modules et de Professeurs
</commit_message>
<xml_diff>
--- a/resources/AP1/modules.xlsx
+++ b/resources/AP1/modules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\AP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1241C2-B758-41C9-9948-FF81D8482126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55EF1FE-CDD7-4DCC-82C2-D60955CDB4C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4C56605D-1814-484D-BD67-6BFC85BD123D}"/>
+    <workbookView xWindow="5115" yWindow="2760" windowWidth="15375" windowHeight="8325" xr2:uid="{4C56605D-1814-484D-BD67-6BFC85BD123D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
     <t>Intitulé</t>
   </si>
   <si>
-    <t>Enseignant</t>
+    <t>Composants</t>
   </si>
   <si>
-    <t>Nombre d'heures</t>
+    <t>Chef  Module</t>
   </si>
 </sst>
 </file>
@@ -391,10 +391,14 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -404,10 +408,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>